<commit_message>
Preenchimento da tabela inicial parcial
</commit_message>
<xml_diff>
--- a/Analyze/planilha-tempo-de-execucao.xlsx
+++ b/Analyze/planilha-tempo-de-execucao.xlsx
@@ -73,12 +73,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="0.0000000"/>
-    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="0.00000000"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.00000000"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="0.000000"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -86,14 +86,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -105,6 +97,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -118,8 +118,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -141,52 +172,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -195,8 +180,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,7 +204,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,11 +225,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -239,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,7 +302,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,121 +422,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,37 +434,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,7 +446,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,6 +488,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -549,30 +533,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -587,22 +547,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,133 +576,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -756,16 +711,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -775,14 +739,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -790,14 +754,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -10840,7 +10804,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>170497</xdr:rowOff>
+      <xdr:rowOff>169545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -10901,16 +10865,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>75247</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>88582</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1021080</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>141922</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>164782</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>141605</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -10918,7 +10882,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8743315" y="427355"/>
+        <a:off x="4887595" y="3308985"/>
         <a:ext cx="5850255" cy="2449830"/>
       </xdr:xfrm>
       <a:graphic>
@@ -11015,7 +10979,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>410527</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>170497</xdr:rowOff>
+      <xdr:rowOff>169545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -11368,8 +11332,8 @@
   <sheetPr/>
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D44" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35"/>
@@ -12266,73 +12230,157 @@
       <c r="A38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="B38" s="16">
+        <v>0.0003646722</v>
+      </c>
+      <c r="C38" s="16">
+        <v>0.0244330261</v>
+      </c>
+      <c r="D38" s="16">
+        <v>2.0326819075</v>
+      </c>
+      <c r="E38" s="16">
+        <v>271.69306284</v>
+      </c>
+      <c r="F38" s="23">
+        <v>29745.6117191</v>
+      </c>
+      <c r="G38" s="16">
+        <v>739743.55642752</v>
+      </c>
+      <c r="H38" s="16">
+        <v>298860.776139345</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="B39" s="16">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C39" s="16">
+        <v>0.006928768</v>
+      </c>
+      <c r="D39" s="16">
+        <v>0.08715661</v>
+      </c>
+      <c r="E39" s="16">
+        <v>1.101309537</v>
+      </c>
+      <c r="F39" s="23">
+        <v>13.8852522983</v>
+      </c>
+      <c r="G39" s="16">
+        <v>72.33087422826</v>
+      </c>
+      <c r="H39" s="16">
+        <v>154.0616471</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
+      <c r="B40" s="16">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="C40" s="16">
+        <v>0.0083874567</v>
+      </c>
+      <c r="D40" s="16">
+        <v>0.1068489054</v>
+      </c>
+      <c r="E40" s="16">
+        <v>1.26541195</v>
+      </c>
+      <c r="F40" s="23">
+        <v>16.926617046</v>
+      </c>
+      <c r="G40" s="16">
+        <v>76.8192576006</v>
+      </c>
+      <c r="H40" s="16">
+        <v>158.270694788249</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
+      <c r="B41" s="16">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C41" s="16">
+        <v>0.00072934459</v>
+      </c>
+      <c r="D41" s="16">
+        <v>0.61811909459</v>
+      </c>
+      <c r="E41" s="16">
+        <v>58.7771088071</v>
+      </c>
+      <c r="F41" s="16">
+        <v>5917.273055477</v>
+      </c>
+      <c r="G41" s="24">
+        <v>139065.63039</v>
+      </c>
+      <c r="H41" s="24">
+        <v>558118.936776</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="B42" s="16">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C42" s="16">
+        <v>0.0069287686</v>
+      </c>
+      <c r="D42" s="16">
+        <v>0.111224969</v>
+      </c>
+      <c r="E42" s="16">
+        <v>1.789445662043</v>
+      </c>
+      <c r="F42" s="16">
+        <v>43.34564709228</v>
+      </c>
+      <c r="G42" s="16">
+        <v>923.6486166166</v>
+      </c>
+      <c r="H42" s="16">
+        <v>3940.740794766</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
+      <c r="B43" s="16">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="C43" s="16">
+        <v>0.014222209</v>
+      </c>
+      <c r="D43" s="16">
+        <v>1.012694233</v>
+      </c>
+      <c r="E43" s="16">
+        <v>96.020334112515</v>
+      </c>
+      <c r="F43" s="16">
+        <v>9003.37941572246</v>
+      </c>
+      <c r="G43" s="24">
+        <v>224160.39771131</v>
+      </c>
+      <c r="H43" s="24">
+        <v>903981.375821059</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -12402,82 +12450,174 @@
       <c r="D48" s="8">
         <v>1.07031319515656</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
+      <c r="E48" s="5">
+        <v>99.283491868537</v>
+      </c>
+      <c r="F48" s="5">
+        <v>9664.62109818</v>
+      </c>
+      <c r="G48" s="8">
+        <v>245270.455365966</v>
+      </c>
+      <c r="H48" s="8">
+        <v>967866.559841994</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
+      <c r="B49" s="5">
+        <v>0.00036467229817941</v>
+      </c>
+      <c r="C49" s="5">
+        <v>0.00036467</v>
+      </c>
+      <c r="D49" s="8">
+        <v>0.002188033</v>
+      </c>
+      <c r="E49" s="8">
+        <v>0.0207863</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0.20749853766</v>
+      </c>
+      <c r="G49" s="8">
+        <v>1.01707029</v>
+      </c>
+      <c r="H49" s="8">
+        <v>2.146461147</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
+      <c r="B50" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="C50" s="8">
+        <v>0.00765811</v>
+      </c>
+      <c r="D50" s="8">
+        <v>0.7917035593</v>
+      </c>
+      <c r="E50" s="5">
+        <v>59.3376652998</v>
+      </c>
+      <c r="F50" s="5">
+        <v>11124.6650484941</v>
+      </c>
+      <c r="G50" s="8">
+        <v>140101.38903577</v>
+      </c>
+      <c r="H50" s="8">
+        <v>1193754.9044777</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
+      <c r="B51" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="C51" s="8">
+        <v>0.0040113952</v>
+      </c>
+      <c r="D51" s="8">
+        <v>0.0266210777</v>
+      </c>
+      <c r="E51" s="8">
+        <v>0.3650369704</v>
+      </c>
+      <c r="F51" s="8">
+        <v>4.1280904153</v>
+      </c>
+      <c r="G51" s="8">
+        <v>24.222610395</v>
+      </c>
+      <c r="H51" s="8">
+        <v>44.254806745562</v>
+      </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
+      <c r="B52" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="C52" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="D52" s="8">
+        <v>0.002917378385</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0.031361817</v>
+      </c>
+      <c r="F52" s="5">
+        <v>0.3066894</v>
+      </c>
+      <c r="G52" s="8">
+        <v>1.527611142</v>
+      </c>
+      <c r="H52" s="8">
+        <v>3.35206776486</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
+      <c r="B53" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="C53" s="8">
+        <v>0.0021880321</v>
+      </c>
+      <c r="D53" s="8">
+        <v>0.0506894124</v>
+      </c>
+      <c r="E53" s="8">
+        <v>0.27459804025</v>
+      </c>
+      <c r="F53" s="8">
+        <v>2.812715384419</v>
+      </c>
+      <c r="G53" s="5">
+        <v>14.8370463024</v>
+      </c>
+      <c r="H53" s="5">
+        <v>30.0471520937644</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
+      <c r="B54" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="C54" s="8">
+        <v>0.01094016894</v>
+      </c>
+      <c r="D54" s="8">
+        <v>0.995920046</v>
+      </c>
+      <c r="E54" s="5">
+        <v>93.853886</v>
+      </c>
+      <c r="F54" s="5">
+        <v>9437.8098802853</v>
+      </c>
+      <c r="G54" s="5">
+        <v>226727.231519333</v>
+      </c>
+      <c r="H54" s="5">
+        <v>949199.76092084</v>
+      </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
@@ -12533,85 +12673,183 @@
       <c r="A59" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
+      <c r="B59" s="8">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C59" s="8">
+        <v>0.027350422</v>
+      </c>
+      <c r="D59" s="5">
+        <v>2.47904228302</v>
+      </c>
+      <c r="E59" s="8">
+        <v>249.61381203622</v>
+      </c>
+      <c r="F59" s="8">
+        <v>25154.97916262</v>
+      </c>
+      <c r="G59" s="8">
+        <v>597291.35909619</v>
+      </c>
+      <c r="H59" s="8">
+        <v>2347234.46204271</v>
+      </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
+      <c r="B60" s="8">
+        <v>0.0003646722</v>
+      </c>
+      <c r="C60" s="8">
+        <v>0.0361025575</v>
+      </c>
+      <c r="D60" s="8">
+        <v>3.16243816</v>
+      </c>
+      <c r="E60" s="5">
+        <v>243.53071343</v>
+      </c>
+      <c r="F60" s="5">
+        <v>23950.1095475583</v>
+      </c>
+      <c r="G60" s="8">
+        <v>612276.407178204</v>
+      </c>
+      <c r="H60" s="8">
+        <v>2402872.13422274</v>
+      </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
+      <c r="B61" s="8">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C61" s="8">
+        <v>0.0145868919</v>
+      </c>
+      <c r="D61" s="8">
+        <v>1.22931031</v>
+      </c>
+      <c r="E61" s="5">
+        <v>118.001391589</v>
+      </c>
+      <c r="F61" s="5">
+        <v>11270.58101049</v>
+      </c>
+      <c r="G61" s="8">
+        <v>180329.1850674</v>
+      </c>
+      <c r="H61" s="8">
+        <v>1125942.85658021</v>
+      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
+      <c r="B62" s="8">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C62" s="8">
+        <v>0.00437606</v>
+      </c>
+      <c r="D62" s="8">
+        <v>0.02880911155</v>
+      </c>
+      <c r="E62" s="8">
+        <v>0.34935606</v>
+      </c>
+      <c r="F62" s="8">
+        <v>4.2743240069</v>
+      </c>
+      <c r="G62" s="5">
+        <v>23.9582231</v>
+      </c>
+      <c r="H62" s="5">
+        <v>46.170795</v>
+      </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
+      <c r="B63" s="8">
+        <v>0.0003646722</v>
+      </c>
+      <c r="C63" s="8">
+        <v>0.0131282027</v>
+      </c>
+      <c r="D63" s="8">
+        <v>1.1811735738</v>
+      </c>
+      <c r="E63" s="5">
+        <v>115.4023721</v>
+      </c>
+      <c r="F63" s="5">
+        <v>11766.56925054</v>
+      </c>
+      <c r="G63" s="5">
+        <v>279936.685641768</v>
+      </c>
+      <c r="H63" s="5">
+        <v>1180015.54233334</v>
+      </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
+      <c r="B64" s="8">
+        <v>0.0003646722</v>
+      </c>
+      <c r="C64" s="8">
+        <v>0.0003646722</v>
+      </c>
+      <c r="D64" s="8">
+        <v>0.04011392354</v>
+      </c>
+      <c r="E64" s="8">
+        <v>0.9649221972219</v>
+      </c>
+      <c r="F64" s="8">
+        <v>59.8321049963</v>
+      </c>
+      <c r="G64" s="8">
+        <v>2012.665789022</v>
+      </c>
+      <c r="H64" s="8">
+        <v>8268.4390943</v>
+      </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="22"/>
-      <c r="G65" s="21"/>
-      <c r="H65" s="21"/>
+      <c r="B65" s="8">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C65" s="8">
+        <v>0.012398858138</v>
+      </c>
+      <c r="D65" s="8">
+        <v>1.0480681849</v>
+      </c>
+      <c r="E65" s="5">
+        <v>96.008734630885</v>
+      </c>
+      <c r="F65" s="22">
+        <v>11075.3613537802</v>
+      </c>
+      <c r="G65" s="21">
+        <v>240086.623829858</v>
+      </c>
+      <c r="H65" s="21">
+        <v>1004123.06668981</v>
+      </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
@@ -12641,7 +12879,7 @@
   <mergeCells count="1">
     <mergeCell ref="A34:G34"/>
   </mergeCells>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
@@ -12824,7 +13062,7 @@
       <c r="D16" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
@@ -14326,7 +14564,7 @@
       <c r="D16" s="10"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.314583333333333" footer="0.314583333333333"/>
+  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Novas alterações na panilha
</commit_message>
<xml_diff>
--- a/Analyze/planilha-tempo-de-execucao.xlsx
+++ b/Analyze/planilha-tempo-de-execucao.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10766" windowHeight="9259" tabRatio="987"/>
+    <workbookView windowWidth="22202" windowHeight="9728" tabRatio="978" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -745,22 +745,22 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="180" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -10778,7 +10778,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="8418195" y="343535"/>
-        <a:ext cx="5855970" cy="2449830"/>
+        <a:ext cx="6390640" cy="2449830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -10813,7 +10813,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="8388985" y="440690"/>
-        <a:ext cx="7075170" cy="2441575"/>
+        <a:ext cx="7606030" cy="2441575"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -10847,8 +10847,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9128125" y="758825"/>
-        <a:ext cx="5829300" cy="2449830"/>
+        <a:off x="9460865" y="758825"/>
+        <a:ext cx="6027420" cy="2449830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -10865,16 +10865,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1021080</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>276860</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>55880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>141605</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>343535</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -10882,7 +10882,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4887595" y="3308985"/>
+        <a:off x="11127740" y="1581785"/>
         <a:ext cx="5850255" cy="2449830"/>
       </xdr:xfrm>
       <a:graphic>
@@ -10917,8 +10917,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8886190" y="250190"/>
-        <a:ext cx="5852160" cy="2449830"/>
+        <a:off x="9218930" y="250190"/>
+        <a:ext cx="6805295" cy="2449830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -10952,8 +10952,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8846185" y="522605"/>
-        <a:ext cx="5846445" cy="2449830"/>
+        <a:off x="8945245" y="522605"/>
+        <a:ext cx="6044565" cy="2449830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -10987,8 +10987,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8990965" y="271145"/>
-        <a:ext cx="5852160" cy="2441575"/>
+        <a:off x="9228455" y="271145"/>
+        <a:ext cx="6709410" cy="2441575"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -11332,8 +11332,8 @@
   <sheetPr/>
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65:H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35"/>
@@ -11368,7 +11368,7 @@
       <c r="E1" s="1">
         <v>10000</v>
       </c>
-      <c r="F1" s="17">
+      <c r="F1" s="21">
         <v>100000</v>
       </c>
       <c r="G1" s="1">
@@ -11391,21 +11391,21 @@
       <c r="E2" s="5">
         <v>879.92810661</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="22">
         <v>99342.69081771</v>
       </c>
       <c r="G2" s="8">
         <v>10671006.8990172</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
@@ -11423,21 +11423,21 @@
       <c r="E3" s="5">
         <v>908.12799423</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="22">
         <v>102421.3497921</v>
       </c>
       <c r="G3" s="8">
         <v>10227994.7349717</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
@@ -11455,20 +11455,20 @@
       <c r="E4" s="8">
         <v>3.13926025</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="24">
         <v>38.47764052</v>
       </c>
       <c r="G4" s="5">
         <v>502.00196797</v>
       </c>
-      <c r="H4" s="19"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="25"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
       <c r="N4" s="25"/>
-      <c r="O4" s="19"/>
+      <c r="O4" s="23"/>
       <c r="P4" s="25"/>
     </row>
     <row r="5" spans="1:16">
@@ -11487,21 +11487,21 @@
       <c r="E5" s="8">
         <v>3.77386891</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="24">
         <v>42.59147836</v>
       </c>
       <c r="G5" s="5">
         <v>458.47610959</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
@@ -11522,18 +11522,18 @@
       <c r="F6" s="5">
         <v>18256.02525434</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="16">
         <v>2102130.7931026</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="25"/>
-      <c r="K6" s="19"/>
+      <c r="K6" s="23"/>
       <c r="L6" s="25"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
@@ -11557,15 +11557,15 @@
       <c r="G7" s="5">
         <v>883.60746802</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
       <c r="K7" s="25"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
@@ -11586,18 +11586,18 @@
       <c r="F8" s="5">
         <v>32191.3011573</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="16">
         <v>3305599.08683063</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
@@ -11621,15 +11621,15 @@
       <c r="G9" s="5">
         <v>836.49889306</v>
       </c>
-      <c r="H9" s="19"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="25"/>
-      <c r="J9" s="19"/>
+      <c r="J9" s="23"/>
       <c r="K9" s="25"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
@@ -11653,28 +11653,28 @@
       <c r="G10" s="5">
         <v>677.83475286</v>
       </c>
-      <c r="H10" s="19"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="25"/>
-      <c r="J10" s="19"/>
+      <c r="J10" s="23"/>
       <c r="K10" s="25"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
     </row>
     <row r="11" spans="6:16">
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="26"/>
       <c r="J11" s="25"/>
-      <c r="K11" s="19"/>
+      <c r="K11" s="23"/>
       <c r="L11" s="25"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="1" t="s">
@@ -11698,15 +11698,15 @@
       <c r="G12" s="1">
         <v>1000000</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
@@ -11730,15 +11730,15 @@
       <c r="G13" s="8">
         <v>3462956.62466874</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
@@ -11762,15 +11762,15 @@
       <c r="G14" s="8">
         <v>6.68306214</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
@@ -12110,10 +12110,10 @@
       <c r="E30" s="5">
         <v>321.84409401</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F30" s="14">
         <v>33223.17525</v>
       </c>
-      <c r="G30" s="21">
+      <c r="G30" s="16">
         <v>3142924.25278464</v>
       </c>
     </row>
@@ -12164,15 +12164,15 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -12190,7 +12190,7 @@
       <c r="E36" s="1">
         <v>10000</v>
       </c>
-      <c r="F36" s="17">
+      <c r="F36" s="21">
         <v>100000</v>
       </c>
       <c r="G36" s="1">
@@ -12204,25 +12204,25 @@
       <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="13">
         <v>0.00036467229817941</v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="13">
         <v>0.0251623792223405</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="13">
         <v>2.02721182704334</v>
       </c>
-      <c r="E37" s="16">
+      <c r="E37" s="13">
         <v>260.856104062811</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="19">
         <v>29710.6464461251</v>
       </c>
-      <c r="G37" s="16">
+      <c r="G37" s="13">
         <v>746315.855575288</v>
       </c>
-      <c r="H37" s="16">
+      <c r="H37" s="13">
         <v>3014609.04358125</v>
       </c>
     </row>
@@ -12230,25 +12230,25 @@
       <c r="A38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="16">
+      <c r="B38" s="13">
         <v>0.0003646722</v>
       </c>
-      <c r="C38" s="16">
+      <c r="C38" s="13">
         <v>0.0244330261</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="13">
         <v>2.0326819075</v>
       </c>
-      <c r="E38" s="16">
+      <c r="E38" s="13">
         <v>271.69306284</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="19">
         <v>29745.6117191</v>
       </c>
-      <c r="G38" s="16">
+      <c r="G38" s="13">
         <v>739743.55642752</v>
       </c>
-      <c r="H38" s="16">
+      <c r="H38" s="13">
         <v>298860.776139345</v>
       </c>
     </row>
@@ -12256,25 +12256,25 @@
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="16">
+      <c r="B39" s="13">
         <v>0.00072934459</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C39" s="13">
         <v>0.006928768</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="13">
         <v>0.08715661</v>
       </c>
-      <c r="E39" s="16">
+      <c r="E39" s="13">
         <v>1.101309537</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="19">
         <v>13.8852522983</v>
       </c>
-      <c r="G39" s="16">
+      <c r="G39" s="13">
         <v>72.33087422826</v>
       </c>
-      <c r="H39" s="16">
+      <c r="H39" s="13">
         <v>154.0616471</v>
       </c>
     </row>
@@ -12282,25 +12282,25 @@
       <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B40" s="13">
         <v>0.00036467229817</v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="13">
         <v>0.0083874567</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="13">
         <v>0.1068489054</v>
       </c>
-      <c r="E40" s="16">
+      <c r="E40" s="13">
         <v>1.26541195</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="19">
         <v>16.926617046</v>
       </c>
-      <c r="G40" s="16">
+      <c r="G40" s="13">
         <v>76.8192576006</v>
       </c>
-      <c r="H40" s="16">
+      <c r="H40" s="13">
         <v>158.270694788249</v>
       </c>
     </row>
@@ -12308,25 +12308,25 @@
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="13">
         <v>0.00072934459</v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41" s="13">
         <v>0.00072934459</v>
       </c>
-      <c r="D41" s="16">
+      <c r="D41" s="13">
         <v>0.61811909459</v>
       </c>
-      <c r="E41" s="16">
+      <c r="E41" s="13">
         <v>58.7771088071</v>
       </c>
-      <c r="F41" s="16">
+      <c r="F41" s="13">
         <v>5917.273055477</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="15">
         <v>139065.63039</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H41" s="15">
         <v>558118.936776</v>
       </c>
     </row>
@@ -12334,25 +12334,25 @@
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="13">
         <v>0.00072934459</v>
       </c>
-      <c r="C42" s="16">
+      <c r="C42" s="13">
         <v>0.0069287686</v>
       </c>
-      <c r="D42" s="16">
+      <c r="D42" s="13">
         <v>0.111224969</v>
       </c>
-      <c r="E42" s="16">
+      <c r="E42" s="13">
         <v>1.789445662043</v>
       </c>
-      <c r="F42" s="16">
+      <c r="F42" s="13">
         <v>43.34564709228</v>
       </c>
-      <c r="G42" s="16">
+      <c r="G42" s="13">
         <v>923.6486166166</v>
       </c>
-      <c r="H42" s="16">
+      <c r="H42" s="13">
         <v>3940.740794766</v>
       </c>
     </row>
@@ -12360,25 +12360,25 @@
       <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="16">
+      <c r="B43" s="13">
         <v>0.00036467229817</v>
       </c>
-      <c r="C43" s="16">
+      <c r="C43" s="13">
         <v>0.014222209</v>
       </c>
-      <c r="D43" s="16">
+      <c r="D43" s="13">
         <v>1.012694233</v>
       </c>
-      <c r="E43" s="16">
+      <c r="E43" s="13">
         <v>96.020334112515</v>
       </c>
-      <c r="F43" s="16">
+      <c r="F43" s="13">
         <v>9003.37941572246</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G43" s="15">
         <v>224160.39771131</v>
       </c>
-      <c r="H43" s="24">
+      <c r="H43" s="15">
         <v>903981.375821059</v>
       </c>
     </row>
@@ -12386,30 +12386,30 @@
       <c r="A44" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
     </row>
     <row r="46" spans="6:8">
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -12841,13 +12841,13 @@
       <c r="E65" s="5">
         <v>96.008734630885</v>
       </c>
-      <c r="F65" s="22">
+      <c r="F65" s="14">
         <v>11075.3613537802</v>
       </c>
-      <c r="G65" s="21">
+      <c r="G65" s="16">
         <v>240086.623829858</v>
       </c>
-      <c r="H65" s="21">
+      <c r="H65" s="16">
         <v>1004123.06668981</v>
       </c>
     </row>
@@ -12888,10 +12888,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
@@ -13055,11 +13055,19 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>
@@ -13072,19 +13080,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="21.8880597014925"/>
     <col min="2" max="2" width="23.4402985074627" customWidth="1"/>
     <col min="3" max="3" width="23.3283582089552" customWidth="1"/>
     <col min="4" max="4" width="22.5522388059701" customWidth="1"/>
-    <col min="5" max="1025" width="11.3283582089552"/>
+    <col min="5" max="5" width="12.4925373134328"/>
+    <col min="6" max="6" width="14.1194029850746"/>
+    <col min="7" max="8" width="12.4925373134328"/>
+    <col min="9" max="1025" width="11.3283582089552"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -13167,7 +13178,7 @@
       <c r="C6" s="6">
         <v>35107.45241824</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <v>88249.403789</v>
       </c>
     </row>
@@ -13181,7 +13192,7 @@
       <c r="C7" s="6">
         <v>3462956.62466874</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <v>9144960.6452824</v>
       </c>
     </row>
@@ -13203,49 +13214,126 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="13">
+        <v>0.00036467229817941</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.00036467229817941</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.00072934459</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>100</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="13">
+        <v>0.0251623792223405</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.0113048412435617</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.027350422</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>1000</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="B13" s="13">
+        <v>2.02721182704334</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1.07031319515656</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2.47904228302</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>10000</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
+      <c r="B14" s="13">
+        <v>260.856104062811</v>
+      </c>
+      <c r="C14" s="5">
+        <v>99.283491868537</v>
+      </c>
+      <c r="D14" s="8">
+        <v>249.61381203622</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>100000</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="14"/>
+      <c r="B15" s="19">
+        <v>29710.6464461251</v>
+      </c>
+      <c r="C15" s="5">
+        <v>9664.62109818</v>
+      </c>
+      <c r="D15" s="8">
+        <v>25154.97916262</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B16" s="13">
+        <v>746315.855575288</v>
+      </c>
+      <c r="C16" s="8">
+        <v>245270.455365966</v>
+      </c>
+      <c r="D16" s="8">
+        <v>597291.35909619</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>1000000</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="14"/>
+      <c r="B17" s="13">
+        <v>3014609.04358125</v>
+      </c>
+      <c r="C17" s="8">
+        <v>967866.559841994</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2347234.46204271</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="5"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -13261,19 +13349,21 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="22.5522388059701" customWidth="1"/>
     <col min="2" max="2" width="22.3283582089552" customWidth="1"/>
     <col min="3" max="3" width="22.5522388059701" customWidth="1"/>
     <col min="4" max="4" width="22.1119402985075" customWidth="1"/>
-    <col min="5" max="1025" width="11.3283582089552"/>
+    <col min="5" max="5" width="15.2388059701493"/>
+    <col min="6" max="7" width="12.4925373134328"/>
+    <col min="8" max="1025" width="11.3283582089552"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -13392,49 +13482,168 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="13">
+        <v>0.0003646722</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.00036467229817941</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.0003646722</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>100</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="13">
+        <v>0.0244330261</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.00036467</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.0361025575</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>1000</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
+      <c r="B13" s="13">
+        <v>2.0326819075</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.002188033</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3.16243816</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>10000</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="B14" s="13">
+        <v>271.69306284</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.0207863</v>
+      </c>
+      <c r="D14" s="5">
+        <v>243.53071343</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>100000</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="10"/>
+      <c r="B15" s="19">
+        <v>29745.6117191</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.20749853766</v>
+      </c>
+      <c r="D15" s="5">
+        <v>23950.1095475583</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B16" s="13">
+        <v>739743.55642752</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1.01707029</v>
+      </c>
+      <c r="D16" s="8">
+        <v>612276.407178204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>1000000</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="B17" s="13">
+        <v>298860.776139345</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2.146461147</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2402872.13422274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="13">
+        <v>0.0003646722</v>
+      </c>
+      <c r="B22" s="13">
+        <v>0.0244330261</v>
+      </c>
+      <c r="C22" s="13">
+        <v>2.0326819075</v>
+      </c>
+      <c r="D22" s="13">
+        <v>271.69306284</v>
+      </c>
+      <c r="E22" s="19">
+        <v>29745.6117191</v>
+      </c>
+      <c r="F22" s="13">
+        <v>739743.55642752</v>
+      </c>
+      <c r="G22" s="13">
+        <v>298860.776139345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="5">
+        <v>0.00036467229817941</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0.00036467</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.002188033</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.0207863</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.20749853766</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1.01707029</v>
+      </c>
+      <c r="G23" s="8">
+        <v>2.146461147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="8">
+        <v>0.0003646722</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.0361025575</v>
+      </c>
+      <c r="C24" s="8">
+        <v>3.16243816</v>
+      </c>
+      <c r="D24" s="5">
+        <v>243.53071343</v>
+      </c>
+      <c r="E24" s="5">
+        <v>23950.1095475583</v>
+      </c>
+      <c r="F24" s="8">
+        <v>612276.407178204</v>
+      </c>
+      <c r="G24" s="8">
+        <v>2402872.13422274</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -13450,18 +13659,20 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="23.8880597014925"/>
     <col min="2" max="2" width="25.1119402985075" customWidth="1"/>
     <col min="3" max="4" width="22.4402985074627" customWidth="1"/>
-    <col min="5" max="1025" width="11.3283582089552"/>
+    <col min="5" max="5" width="15.2388059701493"/>
+    <col min="6" max="7" width="12.4925373134328"/>
+    <col min="8" max="1025" width="11.3283582089552"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -13580,49 +13791,168 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="13">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.00072934459</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>100</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="13">
+        <v>0.006928768</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.00765811</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.0145868919</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>1000</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
+      <c r="B13" s="13">
+        <v>0.08715661</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.7917035593</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.22931031</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>10000</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="10"/>
+      <c r="B14" s="13">
+        <v>1.101309537</v>
+      </c>
+      <c r="C14" s="5">
+        <v>59.3376652998</v>
+      </c>
+      <c r="D14" s="5">
+        <v>118.001391589</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>100000</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="10"/>
+      <c r="B15" s="19">
+        <v>13.8852522983</v>
+      </c>
+      <c r="C15" s="5">
+        <v>11124.6650484941</v>
+      </c>
+      <c r="D15" s="5">
+        <v>11270.58101049</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B16" s="13">
+        <v>72.33087422826</v>
+      </c>
+      <c r="C16" s="8">
+        <v>140101.38903577</v>
+      </c>
+      <c r="D16" s="8">
+        <v>180329.1850674</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>1000000</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="10"/>
+      <c r="B17" s="13">
+        <v>154.0616471</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1193754.9044777</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1125942.85658021</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="13">
+        <v>0.00072934459</v>
+      </c>
+      <c r="B22" s="13">
+        <v>0.006928768</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.08715661</v>
+      </c>
+      <c r="D22" s="13">
+        <v>1.101309537</v>
+      </c>
+      <c r="E22" s="19">
+        <v>13.8852522983</v>
+      </c>
+      <c r="F22" s="13">
+        <v>72.33087422826</v>
+      </c>
+      <c r="G22" s="13">
+        <v>154.0616471</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.00765811</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.7917035593</v>
+      </c>
+      <c r="D23" s="5">
+        <v>59.3376652998</v>
+      </c>
+      <c r="E23" s="5">
+        <v>11124.6650484941</v>
+      </c>
+      <c r="F23" s="8">
+        <v>140101.38903577</v>
+      </c>
+      <c r="G23" s="8">
+        <v>1193754.9044777</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="8">
+        <v>0.00072934459</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.0145868919</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1.22931031</v>
+      </c>
+      <c r="D24" s="5">
+        <v>118.001391589</v>
+      </c>
+      <c r="E24" s="5">
+        <v>11270.58101049</v>
+      </c>
+      <c r="F24" s="8">
+        <v>180329.1850674</v>
+      </c>
+      <c r="G24" s="8">
+        <v>1125942.85658021</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -13638,19 +13968,22 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="22.8880597014925" customWidth="1"/>
     <col min="2" max="2" width="22.5522388059701" customWidth="1"/>
     <col min="3" max="3" width="22.6641791044776" customWidth="1"/>
     <col min="4" max="4" width="22.4402985074627" customWidth="1"/>
-    <col min="5" max="1025" width="11.3283582089552"/>
+    <col min="5" max="5" width="12.4925373134328"/>
+    <col min="6" max="6" width="11.9925373134328"/>
+    <col min="7" max="7" width="12.4925373134328"/>
+    <col min="8" max="1025" width="11.3283582089552"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -13769,49 +14102,168 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="13">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.00072934459</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>100</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="13">
+        <v>0.0083874567</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.0040113952</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.00437606</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>1000</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
+      <c r="B13" s="13">
+        <v>0.1068489054</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.0266210777</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.02880911155</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>10000</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="7"/>
+      <c r="B14" s="13">
+        <v>1.26541195</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.3650369704</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.34935606</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>100000</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
+      <c r="B15" s="19">
+        <v>16.926617046</v>
+      </c>
+      <c r="C15" s="8">
+        <v>4.1280904153</v>
+      </c>
+      <c r="D15" s="8">
+        <v>4.2743240069</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B16" s="13">
+        <v>76.8192576006</v>
+      </c>
+      <c r="C16" s="8">
+        <v>24.222610395</v>
+      </c>
+      <c r="D16" s="5">
+        <v>23.9582231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>1000000</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="B17" s="13">
+        <v>158.270694788249</v>
+      </c>
+      <c r="C17" s="8">
+        <v>44.254806745562</v>
+      </c>
+      <c r="D17" s="5">
+        <v>46.170795</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="13">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="B21" s="13">
+        <v>0.0083874567</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.1068489054</v>
+      </c>
+      <c r="D21" s="13">
+        <v>1.26541195</v>
+      </c>
+      <c r="E21" s="19">
+        <v>16.926617046</v>
+      </c>
+      <c r="F21" s="13">
+        <v>76.8192576006</v>
+      </c>
+      <c r="G21" s="13">
+        <v>158.270694788249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.0040113952</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0.0266210777</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.3650369704</v>
+      </c>
+      <c r="E22" s="8">
+        <v>4.1280904153</v>
+      </c>
+      <c r="F22" s="8">
+        <v>24.222610395</v>
+      </c>
+      <c r="G22" s="8">
+        <v>44.254806745562</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="8">
+        <v>0.00072934459</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.00437606</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.02880911155</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.34935606</v>
+      </c>
+      <c r="E23" s="8">
+        <v>4.2743240069</v>
+      </c>
+      <c r="F23" s="5">
+        <v>23.9582231</v>
+      </c>
+      <c r="G23" s="5">
+        <v>46.170795</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -13827,19 +14279,22 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="22.8880597014925"/>
     <col min="2" max="2" width="22.5522388059701" customWidth="1"/>
     <col min="3" max="3" width="22.4402985074627" customWidth="1"/>
     <col min="4" max="4" width="22.5522388059701" customWidth="1"/>
-    <col min="5" max="1025" width="11.3283582089552"/>
+    <col min="5" max="5" width="15.2388059701493"/>
+    <col min="6" max="6" width="16.365671641791"/>
+    <col min="7" max="7" width="17.4925373134328"/>
+    <col min="8" max="1025" width="11.3283582089552"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -13958,49 +14413,168 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="B11" s="13">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.000364672</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>100</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="13">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.0131282027</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>1000</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
+      <c r="B13" s="13">
+        <v>0.61811909459</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.002917378385</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.1811735738</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>10000</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="10"/>
+      <c r="B14" s="13">
+        <v>58.7771088071</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.031361817</v>
+      </c>
+      <c r="D14" s="5">
+        <v>115.4023721</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>100000</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="10"/>
+      <c r="B15" s="13">
+        <v>5917.273055477</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.3066894</v>
+      </c>
+      <c r="D15" s="5">
+        <v>11766.56925054</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B16" s="15">
+        <v>139065.63039</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1.527611142</v>
+      </c>
+      <c r="D16" s="5">
+        <v>279936.685641768</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>1000000</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="B17" s="15">
+        <v>558118.936776</v>
+      </c>
+      <c r="C17" s="8">
+        <v>3.35206776486</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1180015.54233334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="13">
+        <v>0.00072934459</v>
+      </c>
+      <c r="B22" s="13">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C22" s="13">
+        <v>0.61811909459</v>
+      </c>
+      <c r="D22" s="13">
+        <v>58.7771088071</v>
+      </c>
+      <c r="E22" s="13">
+        <v>5917.273055477</v>
+      </c>
+      <c r="F22" s="15">
+        <v>139065.63039</v>
+      </c>
+      <c r="G22" s="15">
+        <v>558118.936776</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.002917378385</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.031361817</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.3066894</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1.527611142</v>
+      </c>
+      <c r="G23" s="8">
+        <v>3.35206776486</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="8">
+        <v>0.0003646722</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.0131282027</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1.1811735738</v>
+      </c>
+      <c r="D24" s="5">
+        <v>115.4023721</v>
+      </c>
+      <c r="E24" s="5">
+        <v>11766.56925054</v>
+      </c>
+      <c r="F24" s="5">
+        <v>279936.685641768</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1180015.54233334</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -14016,17 +14590,18 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="4" width="22.6641791044776" customWidth="1"/>
-    <col min="5" max="1025" width="11.3283582089552"/>
+    <col min="5" max="7" width="12.4925373134328"/>
+    <col min="8" max="1025" width="11.3283582089552"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -14053,7 +14628,7 @@
       <c r="C2" s="6">
         <v>0.0012829</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="17">
         <v>0.0012829</v>
       </c>
     </row>
@@ -14067,7 +14642,7 @@
       <c r="C3" s="9">
         <v>0.00555924</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="18">
         <v>0.00940794</v>
       </c>
     </row>
@@ -14081,7 +14656,7 @@
       <c r="C4" s="9">
         <v>0.05131608</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="18">
         <v>0.10904663</v>
       </c>
     </row>
@@ -14095,7 +14670,7 @@
       <c r="C5" s="9">
         <v>0.85056377</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="18">
         <v>1.37227709</v>
       </c>
     </row>
@@ -14109,7 +14684,7 @@
       <c r="C6" s="9">
         <v>11.01884197</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="18">
         <v>16.41515338</v>
       </c>
     </row>
@@ -14123,7 +14698,7 @@
       <c r="C7" s="6">
         <v>124.85733492</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="18">
         <v>187.48110392</v>
       </c>
     </row>
@@ -14145,49 +14720,168 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="12"/>
+      <c r="B11" s="13">
+        <v>0.00072934459</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.000364672</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>100</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="13">
+        <v>0.0069287686</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.0021880321</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.0003646722</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>1000</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="13">
+        <v>0.111224969</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.0506894124</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.04011392354</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>10000</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="13">
+        <v>1.789445662043</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.27459804025</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.9649221972219</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>100000</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="13"/>
+      <c r="B15" s="13">
+        <v>43.34564709228</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2.812715384419</v>
+      </c>
+      <c r="D15" s="8">
+        <v>59.8321049963</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B16" s="13">
+        <v>923.6486166166</v>
+      </c>
+      <c r="C16" s="5">
+        <v>14.8370463024</v>
+      </c>
+      <c r="D16" s="8">
+        <v>2012.665789022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>1000000</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="13"/>
+      <c r="B17" s="13">
+        <v>3940.740794766</v>
+      </c>
+      <c r="C17" s="5">
+        <v>30.0471520937644</v>
+      </c>
+      <c r="D17" s="8">
+        <v>8268.4390943</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="13">
+        <v>0.00072934459</v>
+      </c>
+      <c r="B21" s="13">
+        <v>0.0069287686</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.111224969</v>
+      </c>
+      <c r="D21" s="13">
+        <v>1.789445662043</v>
+      </c>
+      <c r="E21" s="13">
+        <v>43.34564709228</v>
+      </c>
+      <c r="F21" s="13">
+        <v>923.6486166166</v>
+      </c>
+      <c r="G21" s="13">
+        <v>3940.740794766</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.0021880321</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0.0506894124</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.27459804025</v>
+      </c>
+      <c r="E22" s="8">
+        <v>2.812715384419</v>
+      </c>
+      <c r="F22" s="5">
+        <v>14.8370463024</v>
+      </c>
+      <c r="G22" s="5">
+        <v>30.0471520937644</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="8">
+        <v>0.0003646722</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.0003646722</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.04011392354</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.9649221972219</v>
+      </c>
+      <c r="E23" s="8">
+        <v>59.8321049963</v>
+      </c>
+      <c r="F23" s="8">
+        <v>2012.665789022</v>
+      </c>
+      <c r="G23" s="8">
+        <v>8268.4390943</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -14203,17 +14897,19 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="3" width="22.6641791044776" customWidth="1"/>
     <col min="4" max="4" width="22.3283582089552" customWidth="1"/>
-    <col min="5" max="1025" width="11.3283582089552"/>
+    <col min="5" max="5" width="14.1194029850746"/>
+    <col min="6" max="7" width="16.365671641791"/>
+    <col min="8" max="1025" width="11.3283582089552"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -14296,7 +14992,7 @@
       <c r="C6" s="6">
         <v>32220.11948996</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="12">
         <v>33223.17525</v>
       </c>
     </row>
@@ -14310,7 +15006,7 @@
       <c r="C7" s="6">
         <v>3363985.47284973</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="12">
         <v>3142924.25278464</v>
       </c>
     </row>
@@ -14332,49 +15028,168 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="13">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.00072934459</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>100</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="13">
+        <v>0.014222209</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.01094016894</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.012398858138</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>1000</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
+      <c r="B13" s="13">
+        <v>1.012694233</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.995920046</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.0480681849</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>10000</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="10"/>
+      <c r="B14" s="13">
+        <v>96.020334112515</v>
+      </c>
+      <c r="C14" s="5">
+        <v>93.853886</v>
+      </c>
+      <c r="D14" s="5">
+        <v>96.008734630885</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>100000</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="11"/>
+      <c r="B15" s="13">
+        <v>9003.37941572246</v>
+      </c>
+      <c r="C15" s="5">
+        <v>9437.8098802853</v>
+      </c>
+      <c r="D15" s="14">
+        <v>11075.3613537802</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
+        <v>500000</v>
+      </c>
+      <c r="B16" s="15">
+        <v>224160.39771131</v>
+      </c>
+      <c r="C16" s="5">
+        <v>226727.231519333</v>
+      </c>
+      <c r="D16" s="16">
+        <v>240086.623829858</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
         <v>1000000</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="11"/>
+      <c r="B17" s="15">
+        <v>903981.375821059</v>
+      </c>
+      <c r="C17" s="5">
+        <v>949199.76092084</v>
+      </c>
+      <c r="D17" s="16">
+        <v>1004123.06668981</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="13">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="B21" s="13">
+        <v>0.014222209</v>
+      </c>
+      <c r="C21" s="13">
+        <v>1.012694233</v>
+      </c>
+      <c r="D21" s="13">
+        <v>96.020334112515</v>
+      </c>
+      <c r="E21" s="13">
+        <v>9003.37941572246</v>
+      </c>
+      <c r="F21" s="15">
+        <v>224160.39771131</v>
+      </c>
+      <c r="G21" s="15">
+        <v>903981.375821059</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="8">
+        <v>0.000364672</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.01094016894</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0.995920046</v>
+      </c>
+      <c r="D22" s="5">
+        <v>93.853886</v>
+      </c>
+      <c r="E22" s="5">
+        <v>9437.8098802853</v>
+      </c>
+      <c r="F22" s="5">
+        <v>226727.231519333</v>
+      </c>
+      <c r="G22" s="5">
+        <v>949199.76092084</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="8">
+        <v>0.00072934459</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.012398858138</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1.0480681849</v>
+      </c>
+      <c r="D23" s="5">
+        <v>96.008734630885</v>
+      </c>
+      <c r="E23" s="14">
+        <v>11075.3613537802</v>
+      </c>
+      <c r="F23" s="16">
+        <v>240086.623829858</v>
+      </c>
+      <c r="G23" s="16">
+        <v>1004123.06668981</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -14390,10 +15205,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A16" sqref="A16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35" outlineLevelCol="3"/>
@@ -14557,11 +15372,19 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.786805555555556" bottom="0.786805555555556" header="0.313888888888889" footer="0.313888888888889"/>

</xml_diff>

<commit_message>
Finalização da análise de tempo
</commit_message>
<xml_diff>
--- a/Analyze/planilha-tempo-de-execucao.xlsx
+++ b/Analyze/planilha-tempo-de-execucao.xlsx
@@ -73,12 +73,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="0.0000000"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="178" formatCode="0.00000000"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.00000000"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="0.000000"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -103,8 +103,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -117,15 +155,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -140,7 +179,37 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -155,45 +224,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -201,45 +231,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="43">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +314,90 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -326,13 +410,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,109 +470,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,37 +482,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,26 +551,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,6 +568,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -613,6 +604,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -621,160 +630,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -796,16 +790,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2969,7 +2963,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="000,000,000" sourceLinked="1"/>
+        <c:numFmt formatCode="000.000.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5679,7 +5673,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="000,000,000" sourceLinked="1"/>
+        <c:numFmt formatCode="000.000.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -11368,15 +11362,16 @@
   <sheetPr/>
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108:K115"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.35"/>
   <cols>
     <col min="1" max="1" width="21.6641791044776" customWidth="1"/>
     <col min="2" max="2" width="18.1119402985075" customWidth="1"/>
-    <col min="3" max="4" width="18.4402985074627" customWidth="1"/>
+    <col min="3" max="3" width="21.4925373134328" customWidth="1"/>
+    <col min="4" max="4" width="18.4402985074627" customWidth="1"/>
     <col min="5" max="6" width="18.1119402985075" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="19.4402985074627" customWidth="1"/>
@@ -12996,484 +12991,170 @@
         <v>135.265707529899</v>
       </c>
     </row>
-    <row r="82" spans="3:12">
-      <c r="C82" s="1" t="s">
+    <row r="75" spans="1:8">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="1">
         <v>10</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J82" s="1" t="s">
+      <c r="C75" s="1">
+        <v>100</v>
+      </c>
+      <c r="D75" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E75" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F75" s="31">
+        <v>100000</v>
+      </c>
+      <c r="G75" s="1">
+        <v>500000</v>
+      </c>
+      <c r="H75" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K82" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L82" s="1" t="s">
+      <c r="B76" s="12">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="C76" s="12">
+        <v>0.014222209</v>
+      </c>
+      <c r="D76" s="12">
+        <v>1.012694233</v>
+      </c>
+      <c r="E76" s="12">
+        <v>96.020334112515</v>
+      </c>
+      <c r="F76" s="12">
+        <v>9003.37941572246</v>
+      </c>
+      <c r="G76" s="14">
+        <v>224160.39771131</v>
+      </c>
+      <c r="H76" s="14">
+        <v>903981.375821059</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="3:12">
-      <c r="C83" s="1">
+      <c r="B77" s="12">
+        <v>0.00072934459635882</v>
+      </c>
+      <c r="C77" s="12">
+        <v>0.00802278470857234</v>
+      </c>
+      <c r="D77" s="12">
+        <v>0.106848905436895</v>
+      </c>
+      <c r="E77" s="12">
+        <v>1.42696166202925</v>
+      </c>
+      <c r="F77" s="12">
+        <v>18.604473067147</v>
+      </c>
+      <c r="G77" s="12">
+        <v>107.423263887622</v>
+      </c>
+      <c r="H77" s="12">
+        <v>259.052800863543</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1">
         <v>10</v>
       </c>
-      <c r="D83" s="5">
-        <v>0.00036467229817941</v>
-      </c>
-      <c r="E83" s="5">
-        <v>0.00036467229817941</v>
-      </c>
-      <c r="F83" s="8">
-        <v>0.000364672</v>
-      </c>
-      <c r="G83" s="8">
-        <v>0.000364672</v>
-      </c>
-      <c r="H83" s="8">
-        <v>0.000364672</v>
-      </c>
-      <c r="I83" s="8">
-        <v>0.000364672</v>
-      </c>
-      <c r="J83" s="8">
-        <v>0.000364672</v>
-      </c>
-      <c r="K83" s="8">
-        <v>0.00437606757815292</v>
-      </c>
-      <c r="L83" s="5">
+      <c r="B82" s="12">
+        <v>0.00036467229817</v>
+      </c>
+      <c r="C82" s="12">
         <v>0.00072934459635882</v>
       </c>
     </row>
-    <row r="84" spans="3:12">
-      <c r="C84" s="1">
+    <row r="83" spans="1:3">
+      <c r="A83" s="1">
         <v>100</v>
       </c>
-      <c r="D84" s="8">
-        <v>0.0113048412435617</v>
-      </c>
-      <c r="E84" s="5">
-        <v>0.00036467</v>
-      </c>
-      <c r="F84" s="8">
-        <v>0.00765811</v>
-      </c>
-      <c r="G84" s="8">
-        <v>0.0040113952</v>
-      </c>
-      <c r="H84" s="8">
-        <v>0.000364672</v>
-      </c>
-      <c r="I84" s="8">
-        <v>0.0021880321</v>
-      </c>
-      <c r="J84" s="8">
-        <v>0.01094016894</v>
-      </c>
-      <c r="K84" s="8">
-        <v>0.0255270608725587</v>
-      </c>
-      <c r="L84" s="5">
-        <v>0.00765811826176761</v>
-      </c>
-    </row>
-    <row r="85" spans="3:12">
-      <c r="C85" s="1">
+      <c r="B83" s="12">
+        <v>0.014222209</v>
+      </c>
+      <c r="C83" s="12">
+        <v>0.00802278470857234</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1">
         <v>1000</v>
       </c>
-      <c r="D85" s="8">
-        <v>1.07031319515656</v>
-      </c>
-      <c r="E85" s="8">
-        <v>0.002188033</v>
-      </c>
-      <c r="F85" s="8">
-        <v>0.7917035593</v>
-      </c>
-      <c r="G85" s="8">
-        <v>0.0266210777</v>
-      </c>
-      <c r="H85" s="8">
-        <v>0.002917378385</v>
-      </c>
-      <c r="I85" s="8">
-        <v>0.0506894124</v>
-      </c>
-      <c r="J85" s="8">
-        <v>0.995920046</v>
-      </c>
-      <c r="K85" s="8">
-        <v>0.246518473569281</v>
-      </c>
-      <c r="L85" s="8">
-        <v>0.0897093853521348</v>
-      </c>
-    </row>
-    <row r="86" spans="3:12">
-      <c r="C86" s="1">
+      <c r="B84" s="12">
+        <v>1.012694233</v>
+      </c>
+      <c r="C84" s="12">
+        <v>0.106848905436895</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1">
         <v>10000</v>
       </c>
-      <c r="D86" s="5">
-        <v>99.283491868537</v>
-      </c>
-      <c r="E86" s="8">
-        <v>0.0207863</v>
-      </c>
-      <c r="F86" s="5">
-        <v>59.3376652998</v>
-      </c>
-      <c r="G86" s="8">
-        <v>0.3650369704</v>
-      </c>
-      <c r="H86" s="5">
-        <v>0.031361817</v>
-      </c>
-      <c r="I86" s="8">
-        <v>0.27459804025</v>
-      </c>
-      <c r="J86" s="5">
-        <v>93.853886</v>
-      </c>
-      <c r="K86" s="5">
-        <v>1.85909937611863</v>
-      </c>
-      <c r="L86" s="8">
-        <v>1.12829609056709</v>
-      </c>
-    </row>
-    <row r="87" spans="3:12">
-      <c r="C87" s="1">
+      <c r="B85" s="12">
+        <v>96.020334112515</v>
+      </c>
+      <c r="C85" s="12">
+        <v>1.42696166202925</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="31">
         <v>100000</v>
       </c>
-      <c r="D87" s="5">
-        <v>9664.62109818</v>
-      </c>
-      <c r="E87" s="5">
-        <v>0.20749853766</v>
-      </c>
-      <c r="F87" s="5">
-        <v>11124.6650484941</v>
-      </c>
-      <c r="G87" s="8">
-        <v>4.1280904153</v>
-      </c>
-      <c r="H87" s="5">
-        <v>0.3066894</v>
-      </c>
-      <c r="I87" s="8">
-        <v>2.812715384419</v>
-      </c>
-      <c r="J87" s="5">
-        <v>9437.8098802853</v>
-      </c>
-      <c r="K87" s="8">
-        <v>17.6720195697742</v>
-      </c>
-      <c r="L87" s="8">
-        <v>12.5870290439605</v>
-      </c>
-    </row>
-    <row r="88" spans="3:12">
-      <c r="C88" s="1">
+      <c r="B86" s="12">
+        <v>9003.37941572246</v>
+      </c>
+      <c r="C86" s="12">
+        <v>18.604473067147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1">
         <v>500000</v>
       </c>
-      <c r="D88" s="8">
-        <v>245270.455365966</v>
-      </c>
-      <c r="E88" s="8">
-        <v>1.01707029</v>
-      </c>
-      <c r="F88" s="8">
-        <v>140101.38903577</v>
-      </c>
-      <c r="G88" s="8">
-        <v>24.222610395</v>
-      </c>
-      <c r="H88" s="8">
-        <v>1.527611142</v>
-      </c>
-      <c r="I88" s="5">
-        <v>14.8370463024</v>
-      </c>
-      <c r="J88" s="5">
-        <v>226727.231519333</v>
-      </c>
-      <c r="K88" s="5">
-        <v>90.1976157742534</v>
-      </c>
-      <c r="L88" s="5">
-        <v>69.4492358297565</v>
-      </c>
-    </row>
-    <row r="89" spans="3:12">
-      <c r="C89" s="1">
+      <c r="B87" s="14">
+        <v>224160.39771131</v>
+      </c>
+      <c r="C87" s="12">
+        <v>107.423263887622</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1">
         <v>1000000</v>
       </c>
-      <c r="D89" s="8">
-        <v>967866.559841994</v>
-      </c>
-      <c r="E89" s="8">
-        <v>2.146461147</v>
-      </c>
-      <c r="F89" s="8">
-        <v>1193754.9044777</v>
-      </c>
-      <c r="G89" s="8">
-        <v>44.254806745562</v>
-      </c>
-      <c r="H89" s="8">
-        <v>3.35206776486</v>
-      </c>
-      <c r="I89" s="5">
-        <v>30.0471520937644</v>
-      </c>
-      <c r="J89" s="5">
-        <v>949199.76092084</v>
-      </c>
-      <c r="K89" s="5">
-        <v>168.835980611103</v>
-      </c>
-      <c r="L89" s="5">
-        <v>134.479474055024</v>
-      </c>
-    </row>
-    <row r="108" spans="2:11">
-      <c r="B108" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H108" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I108" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J108" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K108" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="109" spans="2:11">
-      <c r="B109" s="1">
-        <v>10</v>
-      </c>
-      <c r="C109" s="8">
-        <v>0.00072934459</v>
-      </c>
-      <c r="D109" s="8">
-        <v>0.0003646722</v>
-      </c>
-      <c r="E109" s="8">
-        <v>0.00072934459</v>
-      </c>
-      <c r="F109" s="8">
-        <v>0.00072934459</v>
-      </c>
-      <c r="G109" s="8">
-        <v>0.0003646722</v>
-      </c>
-      <c r="H109" s="8">
-        <v>0.0003646722</v>
-      </c>
-      <c r="I109" s="8">
-        <v>0.00072934459</v>
-      </c>
-      <c r="J109" s="8">
-        <v>0.0036467229817941</v>
-      </c>
-      <c r="K109" s="8">
-        <v>0.00072934459635882</v>
-      </c>
-    </row>
-    <row r="110" spans="2:11">
-      <c r="B110" s="1">
-        <v>100</v>
-      </c>
-      <c r="C110" s="8">
-        <v>0.027350422</v>
-      </c>
-      <c r="D110" s="8">
-        <v>0.0361025575</v>
-      </c>
-      <c r="E110" s="8">
-        <v>0.0145868919</v>
-      </c>
-      <c r="F110" s="8">
-        <v>0.00437606</v>
-      </c>
-      <c r="G110" s="8">
-        <v>0.0131282027</v>
-      </c>
-      <c r="H110" s="8">
-        <v>0.0003646722</v>
-      </c>
-      <c r="I110" s="8">
-        <v>0.012398858138</v>
-      </c>
-      <c r="J110" s="8">
-        <v>0.0167749257162528</v>
-      </c>
-      <c r="K110" s="8">
-        <v>0.00692877366540879</v>
-      </c>
-    </row>
-    <row r="111" spans="2:11">
-      <c r="B111" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C111" s="5">
-        <v>2.47904228302</v>
-      </c>
-      <c r="D111" s="8">
-        <v>3.16243816</v>
-      </c>
-      <c r="E111" s="8">
-        <v>1.22931031</v>
-      </c>
-      <c r="F111" s="8">
-        <v>0.02880911155</v>
-      </c>
-      <c r="G111" s="8">
-        <v>1.1811735738</v>
-      </c>
-      <c r="H111" s="8">
-        <v>0.04011392354</v>
-      </c>
-      <c r="I111" s="8">
-        <v>1.0480681849</v>
-      </c>
-      <c r="J111" s="8">
-        <v>0.16629056796981</v>
-      </c>
-      <c r="K111" s="8">
-        <v>0.0867920069666995</v>
-      </c>
-    </row>
-    <row r="112" spans="2:11">
-      <c r="B112" s="1">
-        <v>10000</v>
-      </c>
-      <c r="C112" s="8">
-        <v>249.61381203622</v>
-      </c>
-      <c r="D112" s="5">
-        <v>243.53071343</v>
-      </c>
-      <c r="E112" s="5">
-        <v>118.001391589</v>
-      </c>
-      <c r="F112" s="8">
-        <v>0.34935606</v>
-      </c>
-      <c r="G112" s="5">
-        <v>115.4023721</v>
-      </c>
-      <c r="H112" s="8">
-        <v>0.9649221972219</v>
-      </c>
-      <c r="I112" s="5">
-        <v>96.008734630885</v>
-      </c>
-      <c r="J112" s="8">
-        <v>1.86092273760952</v>
-      </c>
-      <c r="K112" s="8">
-        <v>1.18518496908308</v>
-      </c>
-    </row>
-    <row r="113" spans="2:11">
-      <c r="B113" s="1">
-        <v>100000</v>
-      </c>
-      <c r="C113" s="8">
-        <v>25154.97916262</v>
-      </c>
-      <c r="D113" s="5">
-        <v>23950.1095475583</v>
-      </c>
-      <c r="E113" s="5">
-        <v>11270.58101049</v>
-      </c>
-      <c r="F113" s="8">
-        <v>4.2743240069</v>
-      </c>
-      <c r="G113" s="5">
-        <v>11766.56925054</v>
-      </c>
-      <c r="H113" s="8">
-        <v>59.8321049963</v>
-      </c>
-      <c r="I113" s="13">
-        <v>11075.3613537802</v>
-      </c>
-      <c r="J113" s="8">
-        <v>18.0954041079605</v>
-      </c>
-      <c r="K113" s="8">
-        <v>12.6001572466949</v>
-      </c>
-    </row>
-    <row r="114" spans="2:11">
-      <c r="B114" s="1">
-        <v>500000</v>
-      </c>
-      <c r="C114" s="8">
-        <v>597291.35909619</v>
-      </c>
-      <c r="D114" s="8">
-        <v>612276.407178204</v>
-      </c>
-      <c r="E114" s="8">
-        <v>180329.1850674</v>
-      </c>
-      <c r="F114" s="5">
-        <v>23.9582231</v>
-      </c>
-      <c r="G114" s="5">
-        <v>279936.685641768</v>
-      </c>
-      <c r="H114" s="8">
-        <v>2012.665789022</v>
-      </c>
-      <c r="I114" s="15">
-        <v>240086.623829858</v>
-      </c>
-      <c r="J114" s="5">
-        <v>89.1094344301452</v>
-      </c>
-      <c r="K114" s="5">
-        <v>69.9878564213274</v>
+      <c r="B88" s="14">
+        <v>903981.375821059</v>
+      </c>
+      <c r="C88" s="12">
+        <v>259.052800863543</v>
       </c>
     </row>
     <row r="115" spans="2:11">

</xml_diff>